<commit_message>
Small implementation handling 403
</commit_message>
<xml_diff>
--- a/docs/api_forecast.xlsx
+++ b/docs/api_forecast.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ottavio/Documents/Thesis/2022-MSDE-OttavioBuonomo/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ottavio/Documents/USI/Thesis/2022-MSDE-OttavioBuonomo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D12CEC97-2C32-2540-9320-B81AB27BADB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8B8469-F9CA-5D41-AF40-3851E2D1932C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{E6F9025F-5EF4-AA41-AF9F-D77098D8905B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,7 +71,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -386,7 +386,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -418,13 +418,21 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44993</v>
+      </c>
+      <c r="B4">
+        <v>700</v>
+      </c>
+    </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>45078</v>
       </c>
       <c r="B25">
-        <f>_xlfn.FORECAST.LINEAR(A25,B1:B3,A1:A3)</f>
-        <v>50.444029850747029</v>
+        <f>_xlfn.FORECAST.LINEAR(A25,B1:B4,A1:A4)</f>
+        <v>2047.2827868852764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel for forecast
</commit_message>
<xml_diff>
--- a/docs/api_forecast.xlsx
+++ b/docs/api_forecast.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ottavio/Documents/USI/Thesis/2022-MSDE-OttavioBuonomo/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ottavio/Documents/Thesis/2022-MSDE-OttavioBuonomo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5379968D-053A-AC49-9865-32160B5F8325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884C0F0A-5E22-1F4C-BB7D-B4C7B036CF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{E6F9025F-5EF4-AA41-AF9F-D77098D8905B}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>2524 urls</t>
+  </si>
+  <si>
+    <t>800 urls</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -95,7 +98,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -394,7 +397,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,13 +448,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45042</v>
+      </c>
+      <c r="B6">
+        <v>59151</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45043</v>
+      </c>
+      <c r="B7">
+        <v>60269</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>45078</v>
       </c>
       <c r="B25">
-        <f>_xlfn.FORECAST.LINEAR(A25,B1:B5,A1:A5)</f>
-        <v>104778.9337708801</v>
+        <f>_xlfn.FORECAST.LINEAR(A25,B1:B7,A1:A7)</f>
+        <v>98554.83383885771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>